<commit_message>
degrees for C programming tricky quizzes
</commit_message>
<xml_diff>
--- a/Quizzes_degrees .xlsx
+++ b/Quizzes_degrees .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Embeded Systems Diploma\GitHup_Repo\Embedded_System_Online_Diploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{124EF46B-42AF-4D27-949A-6D11D5234D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B983AC2D-03CB-4898-A6D1-70AB35582C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{02E31436-80A3-4A05-8D70-D70136B8E901}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Quiz subject</t>
   </si>
@@ -50,13 +50,31 @@
   </si>
   <si>
     <t>48 / 60</t>
+  </si>
+  <si>
+    <t>C Loops &amp; Condition QUIZ</t>
+  </si>
+  <si>
+    <t>34 / 36</t>
+  </si>
+  <si>
+    <t>Array &amp; String</t>
+  </si>
+  <si>
+    <t>32 / 40</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>29 / 34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,16 +106,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF050505"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -118,14 +164,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,90 +499,110 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="26" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="3" max="26" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+    <row r="2" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+    <row r="3" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>